<commit_message>
m coi thử đoạn trên nha
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Tổng thống Mỹ ký ban hành luật TPA, mở đường cho TPP</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Quảng Ninh "nhượng bộ", đền bù đợt 1 cho CTCP Quốc tế Hoàng Gia (RIC) 110 tỷ đồng</t>
   </si>
   <si>
+    <t>VPBS tiếp tục giải chấp thêm cổ phiếu JVC của ông Lê Văn Hướng</t>
+  </si>
+  <si>
     <t>Công ty chứng khoán được mở room 100% ngay</t>
   </si>
   <si>
@@ -37,7 +40,25 @@
     <t>Từ hôm nay (1/7) Luật nhà ở, Luật kinh doanh BĐS 2014 chính thức có hiệu lực</t>
   </si>
   <si>
-    <t>Tổng công ty Tín Nghĩa nhận “cái tát” từ bất động sản</t>
+    <t>Nhịp đập Thị trường 01/07: Thanh khoản sụt giảm mạnh</t>
+  </si>
+  <si>
+    <t>JVC: Ông Lê Văn Hướng tiếp tục bị bán giải chấp</t>
+  </si>
+  <si>
+    <t>Vì sao HHS giảm sàn?</t>
+  </si>
+  <si>
+    <t>Những khoản cổ tức chốt quyền trong nửa đầu tháng 7</t>
+  </si>
+  <si>
+    <t>PMI sản xuất tháng 6 giảm nhưng vẫn duy trì trên mốc 50 điểm</t>
+  </si>
+  <si>
+    <t>Nhịp đập Thị trường 01/07: Tiền chuyển hướng qua một số cổ phiếu nhỏ</t>
+  </si>
+  <si>
+    <t>Hy Lạp vỡ nợ, EU từ chối cứu trợ</t>
   </si>
 </sst>
 </file>
@@ -374,7 +395,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -399,27 +420,72 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>